<commit_message>
Updated all documentation, and added Sprint 3 Backlog
</commit_message>
<xml_diff>
--- a/ProductBacklog.xlsx
+++ b/ProductBacklog.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timbe\Desktop\CS\Classes\Spring2018\SoftwareEngineering2\Stuff\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C68424-8ADE-466C-B486-F0072A6B7212}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{43D5F773-D2B5-4EA8-ADF4-D8B1960A2E1B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6770" xr2:uid="{BE81A106-BA93-4CD3-AA8D-9E16CD4FDDEA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16335" windowHeight="10470" xr2:uid="{BE81A106-BA93-4CD3-AA8D-9E16CD4FDDEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="53">
   <si>
     <t>As a/an</t>
   </si>
@@ -163,6 +159,27 @@
   </si>
   <si>
     <t>I can see any errors in my code</t>
+  </si>
+  <si>
+    <t>have a complete game</t>
+  </si>
+  <si>
+    <t>I can finally play</t>
+  </si>
+  <si>
+    <t>with online highscores</t>
+  </si>
+  <si>
+    <t>have clean and tidy final code</t>
+  </si>
+  <si>
+    <t>my work may be reviewed favorably</t>
+  </si>
+  <si>
+    <t>have all my fellow players share a scoreboard with me on a server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I may compare my skills </t>
   </si>
 </sst>
 </file>
@@ -538,21 +555,21 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="25.953125" customWidth="1"/>
-    <col min="4" max="4" width="27.08984375" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" customWidth="1"/>
-    <col min="6" max="6" width="9.76953125" customWidth="1"/>
-    <col min="7" max="7" width="9.7265625" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -575,7 +592,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="29.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -598,7 +615,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="29.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -619,7 +636,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -640,7 +657,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -661,7 +678,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -682,7 +699,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
@@ -703,7 +720,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="29.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -726,7 +743,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="29.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
@@ -747,7 +764,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -768,7 +785,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -789,7 +806,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
@@ -812,7 +829,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
@@ -833,7 +850,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
@@ -854,34 +871,72 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="F17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -890,7 +945,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -899,7 +954,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="5"/>
@@ -908,7 +963,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -917,7 +972,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -926,7 +981,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -935,7 +990,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -944,7 +999,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -953,7 +1008,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -962,7 +1017,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -971,7 +1026,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>

</xml_diff>